<commit_message>
fix: Regenerate complete Excel file with all 11 sheets
Pricing Data Excel now includes:
- Materials, Series, Body/Bonnet/Plug/Seat/Cage Weights
- Seal Ring Prices, Stem Fixed Prices
- Actuator Models, Handwheel Prices
</commit_message>
<xml_diff>
--- a/templates/Unicorn_Valves_Machining_Costs.xlsx
+++ b/templates/Unicorn_Valves_Machining_Costs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -456,7 +456,7 @@
         <v>91000</v>
       </c>
       <c r="C3" t="str">
-        <v>1</v>
+        <v>1/2</v>
       </c>
       <c r="D3" t="str">
         <v>150</v>
@@ -465,15 +465,15 @@
         <v>Flanged</v>
       </c>
       <c r="F3" t="str">
-        <v>Stainless Steel SS316</v>
+        <v>Stainless Steel SS304</v>
       </c>
       <c r="G3" t="str">
-        <v>4000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Bonnet</v>
+        <v>Body</v>
       </c>
       <c r="B4" t="str">
         <v>91000</v>
@@ -485,87 +485,1099 @@
         <v>150</v>
       </c>
       <c r="E4" t="str">
-        <v>Standard</v>
+        <v>Threaded</v>
       </c>
       <c r="F4" t="str">
         <v>Stainless Steel SS316</v>
       </c>
       <c r="G4" t="str">
-        <v>1500</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Plug</v>
+        <v>Body</v>
       </c>
       <c r="B5" t="str">
         <v>91000</v>
       </c>
       <c r="C5" t="str">
-        <v>1/2</v>
+        <v>3/4</v>
       </c>
       <c r="D5" t="str">
         <v>150</v>
       </c>
       <c r="E5" t="str">
-        <v>Metal Seated</v>
+        <v>Flanged</v>
       </c>
       <c r="F5" t="str">
-        <v>SS316 Plug</v>
+        <v>Stainless Steel SS316</v>
       </c>
       <c r="G5" t="str">
-        <v>1200</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Seat</v>
+        <v>Body</v>
       </c>
       <c r="B6" t="str">
         <v>91000</v>
       </c>
       <c r="C6" t="str">
-        <v>1/2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="str">
         <v>150</v>
       </c>
       <c r="E6" t="str">
-        <v>Metal Seated</v>
+        <v>Flanged</v>
       </c>
       <c r="F6" t="str">
-        <v>SS316 Seat</v>
+        <v>Stainless Steel SS316</v>
       </c>
       <c r="G6" t="str">
-        <v>1000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
+        <v>Body</v>
+      </c>
+      <c r="B7" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C7" t="str">
+        <v>1-1/2</v>
+      </c>
+      <c r="D7" t="str">
+        <v>150</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Flanged</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G7" t="str">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Body</v>
+      </c>
+      <c r="B8" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2</v>
+      </c>
+      <c r="D8" t="str">
+        <v>150</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Flanged</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G8" t="str">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Body</v>
+      </c>
+      <c r="B9" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C9" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D9" t="str">
+        <v>150</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Flanged</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G9" t="str">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Body</v>
+      </c>
+      <c r="B10" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C10" t="str">
+        <v>1</v>
+      </c>
+      <c r="D10" t="str">
+        <v>150</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Flanged</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G10" t="str">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Body</v>
+      </c>
+      <c r="B11" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2</v>
+      </c>
+      <c r="D11" t="str">
+        <v>150</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Flanged</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G11" t="str">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Bonnet</v>
+      </c>
+      <c r="B12" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C12" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D12" t="str">
+        <v>150</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G12" t="str">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Bonnet</v>
+      </c>
+      <c r="B13" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C13" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D13" t="str">
+        <v>150</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Extended</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G13" t="str">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Bonnet</v>
+      </c>
+      <c r="B14" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C14" t="str">
+        <v>3/4</v>
+      </c>
+      <c r="D14" t="str">
+        <v>150</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G14" t="str">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Bonnet</v>
+      </c>
+      <c r="B15" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C15" t="str">
+        <v>1</v>
+      </c>
+      <c r="D15" t="str">
+        <v>150</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G15" t="str">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Bonnet</v>
+      </c>
+      <c r="B16" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C16" t="str">
+        <v>1-1/2</v>
+      </c>
+      <c r="D16" t="str">
+        <v>150</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G16" t="str">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Bonnet</v>
+      </c>
+      <c r="B17" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2</v>
+      </c>
+      <c r="D17" t="str">
+        <v>150</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G17" t="str">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Bonnet</v>
+      </c>
+      <c r="B18" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C18" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D18" t="str">
+        <v>150</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G18" t="str">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Bonnet</v>
+      </c>
+      <c r="B19" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C19" t="str">
+        <v>1</v>
+      </c>
+      <c r="D19" t="str">
+        <v>150</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G19" t="str">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Bonnet</v>
+      </c>
+      <c r="B20" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C20" t="str">
+        <v>2</v>
+      </c>
+      <c r="D20" t="str">
+        <v>150</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Stainless Steel SS316</v>
+      </c>
+      <c r="G20" t="str">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Plug</v>
+      </c>
+      <c r="B21" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C21" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D21" t="str">
+        <v>150</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F21" t="str">
+        <v>SS316 Plug</v>
+      </c>
+      <c r="G21" t="str">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Plug</v>
+      </c>
+      <c r="B22" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C22" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D22" t="str">
+        <v>150</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Soft Seated</v>
+      </c>
+      <c r="F22" t="str">
+        <v>SS316 Plug</v>
+      </c>
+      <c r="G22" t="str">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Plug</v>
+      </c>
+      <c r="B23" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C23" t="str">
+        <v>3/4</v>
+      </c>
+      <c r="D23" t="str">
+        <v>150</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F23" t="str">
+        <v>SS316 Plug</v>
+      </c>
+      <c r="G23" t="str">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Plug</v>
+      </c>
+      <c r="B24" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C24" t="str">
+        <v>1</v>
+      </c>
+      <c r="D24" t="str">
+        <v>150</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F24" t="str">
+        <v>SS316 Plug</v>
+      </c>
+      <c r="G24" t="str">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Plug</v>
+      </c>
+      <c r="B25" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C25" t="str">
+        <v>1-1/2</v>
+      </c>
+      <c r="D25" t="str">
+        <v>150</v>
+      </c>
+      <c r="E25" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F25" t="str">
+        <v>SS316 Plug</v>
+      </c>
+      <c r="G25" t="str">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Plug</v>
+      </c>
+      <c r="B26" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C26" t="str">
+        <v>2</v>
+      </c>
+      <c r="D26" t="str">
+        <v>150</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F26" t="str">
+        <v>SS316 Plug</v>
+      </c>
+      <c r="G26" t="str">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Plug</v>
+      </c>
+      <c r="B27" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C27" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D27" t="str">
+        <v>150</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F27" t="str">
+        <v>SS316 Plug</v>
+      </c>
+      <c r="G27" t="str">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Plug</v>
+      </c>
+      <c r="B28" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C28" t="str">
+        <v>1</v>
+      </c>
+      <c r="D28" t="str">
+        <v>150</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F28" t="str">
+        <v>SS316 Plug</v>
+      </c>
+      <c r="G28" t="str">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Plug</v>
+      </c>
+      <c r="B29" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C29" t="str">
+        <v>2</v>
+      </c>
+      <c r="D29" t="str">
+        <v>150</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F29" t="str">
+        <v>SS316 Plug</v>
+      </c>
+      <c r="G29" t="str">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="B30" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C30" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D30" t="str">
+        <v>150</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F30" t="str">
+        <v>SS316 Seat</v>
+      </c>
+      <c r="G30" t="str">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="B31" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C31" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D31" t="str">
+        <v>150</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Soft Seated</v>
+      </c>
+      <c r="F31" t="str">
+        <v>SS316 Seat</v>
+      </c>
+      <c r="G31" t="str">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="B32" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C32" t="str">
+        <v>3/4</v>
+      </c>
+      <c r="D32" t="str">
+        <v>150</v>
+      </c>
+      <c r="E32" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F32" t="str">
+        <v>SS316 Seat</v>
+      </c>
+      <c r="G32" t="str">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="B33" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C33" t="str">
+        <v>1</v>
+      </c>
+      <c r="D33" t="str">
+        <v>150</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F33" t="str">
+        <v>SS316 Seat</v>
+      </c>
+      <c r="G33" t="str">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="B34" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C34" t="str">
+        <v>1-1/2</v>
+      </c>
+      <c r="D34" t="str">
+        <v>150</v>
+      </c>
+      <c r="E34" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F34" t="str">
+        <v>SS316 Seat</v>
+      </c>
+      <c r="G34" t="str">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="B35" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C35" t="str">
+        <v>2</v>
+      </c>
+      <c r="D35" t="str">
+        <v>150</v>
+      </c>
+      <c r="E35" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F35" t="str">
+        <v>SS316 Seat</v>
+      </c>
+      <c r="G35" t="str">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="B36" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C36" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D36" t="str">
+        <v>150</v>
+      </c>
+      <c r="E36" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F36" t="str">
+        <v>SS316 Seat</v>
+      </c>
+      <c r="G36" t="str">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="B37" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C37" t="str">
+        <v>1</v>
+      </c>
+      <c r="D37" t="str">
+        <v>150</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F37" t="str">
+        <v>SS316 Seat</v>
+      </c>
+      <c r="G37" t="str">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Seat</v>
+      </c>
+      <c r="B38" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C38" t="str">
+        <v>2</v>
+      </c>
+      <c r="D38" t="str">
+        <v>150</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Metal Seated</v>
+      </c>
+      <c r="F38" t="str">
+        <v>SS316 Seat</v>
+      </c>
+      <c r="G38" t="str">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
         <v>Stem</v>
       </c>
-      <c r="B7" t="str">
-        <v>91000</v>
-      </c>
-      <c r="C7" t="str">
-        <v>1/2</v>
-      </c>
-      <c r="D7" t="str">
-        <v>150</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Standard</v>
-      </c>
-      <c r="F7" t="str">
+      <c r="B39" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C39" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D39" t="str">
+        <v>150</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F39" t="str">
         <v>SS316 Stem</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G39" t="str">
         <v>800</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Stem</v>
+      </c>
+      <c r="B40" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C40" t="str">
+        <v>3/4</v>
+      </c>
+      <c r="D40" t="str">
+        <v>150</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F40" t="str">
+        <v>SS316 Stem</v>
+      </c>
+      <c r="G40" t="str">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Stem</v>
+      </c>
+      <c r="B41" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C41" t="str">
+        <v>1</v>
+      </c>
+      <c r="D41" t="str">
+        <v>150</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F41" t="str">
+        <v>SS316 Stem</v>
+      </c>
+      <c r="G41" t="str">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Stem</v>
+      </c>
+      <c r="B42" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C42" t="str">
+        <v>1-1/2</v>
+      </c>
+      <c r="D42" t="str">
+        <v>150</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F42" t="str">
+        <v>SS316 Stem</v>
+      </c>
+      <c r="G42" t="str">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Stem</v>
+      </c>
+      <c r="B43" t="str">
+        <v>91000</v>
+      </c>
+      <c r="C43" t="str">
+        <v>2</v>
+      </c>
+      <c r="D43" t="str">
+        <v>150</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F43" t="str">
+        <v>SS316 Stem</v>
+      </c>
+      <c r="G43" t="str">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Stem</v>
+      </c>
+      <c r="B44" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C44" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D44" t="str">
+        <v>150</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F44" t="str">
+        <v>SS316 Stem</v>
+      </c>
+      <c r="G44" t="str">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Stem</v>
+      </c>
+      <c r="B45" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C45" t="str">
+        <v>1</v>
+      </c>
+      <c r="D45" t="str">
+        <v>150</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F45" t="str">
+        <v>SS316 Stem</v>
+      </c>
+      <c r="G45" t="str">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Stem</v>
+      </c>
+      <c r="B46" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C46" t="str">
+        <v>2</v>
+      </c>
+      <c r="D46" t="str">
+        <v>150</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F46" t="str">
+        <v>SS316 Stem</v>
+      </c>
+      <c r="G46" t="str">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Cage</v>
+      </c>
+      <c r="B47" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C47" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D47" t="str">
+        <v>150</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F47" t="str">
+        <v>SS316 Cage</v>
+      </c>
+      <c r="G47" t="str">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Cage</v>
+      </c>
+      <c r="B48" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C48" t="str">
+        <v>1</v>
+      </c>
+      <c r="D48" t="str">
+        <v>150</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F48" t="str">
+        <v>SS316 Cage</v>
+      </c>
+      <c r="G48" t="str">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Cage</v>
+      </c>
+      <c r="B49" t="str">
+        <v>92000</v>
+      </c>
+      <c r="C49" t="str">
+        <v>2</v>
+      </c>
+      <c r="D49" t="str">
+        <v>150</v>
+      </c>
+      <c r="E49" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F49" t="str">
+        <v>SS316 Cage</v>
+      </c>
+      <c r="G49" t="str">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Cage</v>
+      </c>
+      <c r="B50" t="str">
+        <v>93000</v>
+      </c>
+      <c r="C50" t="str">
+        <v>1/2</v>
+      </c>
+      <c r="D50" t="str">
+        <v>150</v>
+      </c>
+      <c r="E50" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F50" t="str">
+        <v>SS316 Cage</v>
+      </c>
+      <c r="G50" t="str">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Cage</v>
+      </c>
+      <c r="B51" t="str">
+        <v>93000</v>
+      </c>
+      <c r="C51" t="str">
+        <v>1</v>
+      </c>
+      <c r="D51" t="str">
+        <v>150</v>
+      </c>
+      <c r="E51" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="F51" t="str">
+        <v>SS316 Cage</v>
+      </c>
+      <c r="G51" t="str">
+        <v>2700</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G51"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>